<commit_message>
Plotting transition rates for 1k model results (fixed plot labels), formatting new artiodactyla data, comparing Cox artio data to new data. June 13th
</commit_message>
<xml_diff>
--- a/Maor_diel_activity_data.xlsx
+++ b/Maor_diel_activity_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameli\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d80fae471b4ed02/Documents/R_projects/fish_sleep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B92939-F742-4B99-9A53-5A13DEC52CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{E4B92939-F742-4B99-9A53-5A13DEC52CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0690F31A-2DBC-4A26-BAE6-3963A75C5D26}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12079,12 +12079,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I3514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3247" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="25.7265625" customWidth="1"/>
+    <col min="3" max="3" width="36" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>